<commit_message>
Feat: add native API host
- cl::enqueueMapBuffer DOSENOT work, so move to native API
</commit_message>
<xml_diff>
--- a/fpl20_results.xlsx
+++ b/fpl20_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbshi/Workspace/fpl20ext/fpga/udf_op/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D141C09-0DCD-554E-8261-83685D027AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85151EAA-32EF-DA47-8965-4699F5B95E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="988" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="1500" windowWidth="33600" windowHeight="21000" tabRatio="988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ubenchmark" sheetId="1" r:id="rId1"/>
@@ -17747,7 +17747,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>308520</xdr:colOff>
+      <xdr:colOff>308519</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
@@ -17783,7 +17783,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>373320</xdr:colOff>
+      <xdr:colOff>373319</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
@@ -23821,13 +23821,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="83.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" style="2"/>
     <col min="3" max="3" width="18.1640625" style="2"/>
     <col min="4" max="4" width="18.1640625" style="2" customWidth="1"/>
@@ -25425,7 +25425,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26434,7 +26434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -26997,7 +26997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R82"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Feat: udf_ml perf data collection
</commit_message>
<xml_diff>
--- a/fpl20_results.xlsx
+++ b/fpl20_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbshi/Workspace/fpl20ext/fpga/udf_op/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4839DD85-D1D0-994A-8021-1B8A2366D62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109AD6C5-BF1E-BC40-B716-B1375B568B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="988" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="988" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ubenchmark" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="155">
   <si>
     <t>Bandwidth (300 MHz)</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>FPGA-Lcopy-Time (#k=12)</t>
+  </si>
+  <si>
+    <t>dataset (with syn)</t>
   </si>
 </sst>
 </file>
@@ -18031,13 +18034,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>478080</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>151560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>180721</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26540,8 +26543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L112" sqref="L112"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L102" sqref="L102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28895,10 +28898,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R82"/>
+  <dimension ref="A1:R103"/>
   <sheetViews>
-    <sheetView topLeftCell="C36" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28911,9 +28914,10 @@
     <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="53" style="2"/>
-    <col min="9" max="10" width="17.5" style="2"/>
+    <col min="9" max="9" width="19.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="2" customWidth="1"/>
     <col min="11" max="11" width="30.33203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" style="2"/>
+    <col min="12" max="12" width="21.1640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="20.83203125" style="2"/>
     <col min="14" max="14" width="23.6640625" style="2"/>
     <col min="15" max="15" width="10.5" style="2"/>
@@ -29502,1014 +29506,1450 @@
         <v>12.744710077151334</v>
       </c>
     </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>116</v>
-      </c>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K19" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H20" s="2" t="s">
-        <v>119</v>
+        <v>49</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2">
-        <v>0.693326</v>
+        <v>109</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H21" s="2" t="s">
-        <v>122</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20000</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2048</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="2">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2">
+        <f>B21*C21*4/1000000</f>
+        <v>163.84</v>
+      </c>
+      <c r="G21" s="2">
+        <f>J21</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <f>E$21*F$21*G21/1000</f>
+        <v>1.6384000000000001</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
       </c>
       <c r="K21" s="2">
-        <v>8.4084800000000005E-4</v>
+        <v>0.124334</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" ref="L21:L29" si="2">0.770402*J21/10</f>
-        <v>7.7040200000000003E-2</v>
+        <v>0.12431300000000001</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" ref="M21:M29" si="3">J21*3.3942/10</f>
-        <v>0.33942</v>
+        <f>$I21/K21</f>
+        <v>13.177409236411602</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" ref="N21:N29" si="4">0.747845/10*J21</f>
-        <v>7.4784500000000004E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H22" s="2" t="s">
-        <v>123</v>
+        <f>$I21/L21</f>
+        <v>13.179635275474006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G22" s="2">
+        <f t="shared" ref="G22:G24" si="2">J22</f>
+        <v>2</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" ref="I22:I25" si="3">E$21*F$21*G22/1000</f>
+        <v>3.2768000000000002</v>
       </c>
       <c r="J22" s="2">
         <v>2</v>
       </c>
       <c r="K22" s="2">
+        <v>0.12428</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.247729</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" ref="M22:M25" si="4">$I22/K22</f>
+        <v>26.36626971355005</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" ref="N22:N25" si="5">$I22/L22</f>
+        <v>13.227357313838914</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G23" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="3"/>
+        <v>6.5536000000000003</v>
+      </c>
+      <c r="J23" s="2">
+        <v>4</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.124352</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.49914199999999997</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="4"/>
+        <v>52.702007205352551</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="5"/>
+        <v>13.129730617740043</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="3"/>
+        <v>13.107200000000001</v>
+      </c>
+      <c r="J24" s="2">
+        <v>8</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.12515699999999999</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.99620699999999995</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="4"/>
+        <v>104.72606406353621</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="5"/>
+        <v>13.157104898881459</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G25" s="2">
+        <f>J25</f>
+        <v>16</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="3"/>
+        <v>26.214400000000001</v>
+      </c>
+      <c r="J25" s="2">
+        <v>16</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.12601999999999999</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1.9948600000000001</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="4"/>
+        <v>208.01777495635616</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="5"/>
+        <v>13.140972298807936</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="2">
+        <v>20000</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2048</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="2">
+        <v>10</v>
+      </c>
+      <c r="F30" s="2">
+        <f>B30*C30*4/1000000</f>
+        <v>163.84</v>
+      </c>
+      <c r="G30" s="2">
+        <f>J30</f>
+        <v>16</v>
+      </c>
+      <c r="I30" s="2">
+        <f>E30*F30*G30/1000</f>
+        <v>26.214400000000001</v>
+      </c>
+      <c r="J30" s="2">
+        <v>16</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.12601999999999999</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1.9948600000000001</v>
+      </c>
+      <c r="M30" s="2">
+        <f>$I30/K30</f>
+        <v>208.01777495635616</v>
+      </c>
+      <c r="N30" s="2">
+        <f>$I30/L30</f>
+        <v>13.140972298807936</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="2">
+        <v>50000</v>
+      </c>
+      <c r="C31" s="2">
+        <v>784</v>
+      </c>
+      <c r="D31" s="2">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2">
+        <v>10</v>
+      </c>
+      <c r="F31" s="2">
+        <f>B31*C31*4/1000000</f>
+        <v>156.80000000000001</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" ref="G31:G33" si="6">J31</f>
+        <v>16</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" ref="I31:I33" si="7">E31*F31*G31/1000</f>
+        <v>25.088000000000001</v>
+      </c>
+      <c r="J31" s="2">
+        <v>16</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.125995</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1.90964</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" ref="M31:M34" si="8">$I31/K31</f>
+        <v>199.11901265923251</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" ref="N31:N34" si="9">$I31/L31</f>
+        <v>13.137554722356047</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="2">
+        <v>32768</v>
+      </c>
+      <c r="C32" s="2">
+        <v>126</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+      <c r="F32" s="2">
+        <f>B32*C32*4/1000000</f>
+        <v>16.515072</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="7"/>
+        <v>2.64241152</v>
+      </c>
+      <c r="J32" s="2">
+        <v>16</v>
+      </c>
+      <c r="K32" s="2">
+        <v>2.4300100000000002E-2</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0.205822</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="8"/>
+        <v>108.74076732194517</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="9"/>
+        <v>12.838333705823478</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="2">
+        <v>200000</v>
+      </c>
+      <c r="C33" s="2">
+        <v>256</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="2">
+        <v>10</v>
+      </c>
+      <c r="F33" s="2">
+        <f>B33*C33*4/1000000</f>
+        <v>204.8</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="7"/>
+        <v>32.768000000000001</v>
+      </c>
+      <c r="J33" s="2">
+        <v>16</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0.215306</v>
+      </c>
+      <c r="L33" s="2">
+        <v>2.5045999999999999</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="8"/>
+        <v>152.19269319015726</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="9"/>
+        <v>13.083127046234928</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2">
+        <v>0.693326</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H42" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J42" s="2">
+        <v>1</v>
+      </c>
+      <c r="K42" s="2">
+        <v>8.4084800000000005E-4</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" ref="L42:L50" si="10">0.770402*J42/10</f>
+        <v>7.7040200000000003E-2</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" ref="M42:M50" si="11">J42*3.3942/10</f>
+        <v>0.33942</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" ref="N42:N50" si="12">0.747845/10*J42</f>
+        <v>7.4784500000000004E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J43" s="2">
+        <v>2</v>
+      </c>
+      <c r="K43" s="2">
         <v>4.3118799999999999E-4</v>
       </c>
-      <c r="L22" s="2">
-        <f t="shared" si="2"/>
+      <c r="L43" s="2">
+        <f t="shared" si="10"/>
         <v>0.15408040000000001</v>
       </c>
-      <c r="M22" s="2">
-        <f t="shared" si="3"/>
+      <c r="M43" s="2">
+        <f t="shared" si="11"/>
         <v>0.67884</v>
       </c>
-      <c r="N22" s="2">
-        <f t="shared" si="4"/>
+      <c r="N43" s="2">
+        <f t="shared" si="12"/>
         <v>0.14956900000000001</v>
       </c>
     </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="J23" s="2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J44" s="2">
         <v>3</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K44" s="2">
         <v>2.9157500000000003E-4</v>
       </c>
-      <c r="L23" s="2">
-        <f t="shared" si="2"/>
+      <c r="L44" s="2">
+        <f t="shared" si="10"/>
         <v>0.23112060000000004</v>
       </c>
-      <c r="M23" s="2">
-        <f t="shared" si="3"/>
+      <c r="M44" s="2">
+        <f t="shared" si="11"/>
         <v>1.0182600000000002</v>
       </c>
-      <c r="N23" s="2">
-        <f t="shared" si="4"/>
+      <c r="N44" s="2">
+        <f t="shared" si="12"/>
         <v>0.22435350000000001</v>
       </c>
     </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="J24" s="2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J45" s="2">
         <v>4</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K45" s="2">
         <v>2.2086E-4</v>
       </c>
-      <c r="L24" s="2">
-        <f t="shared" si="2"/>
+      <c r="L45" s="2">
+        <f t="shared" si="10"/>
         <v>0.30816080000000001</v>
       </c>
-      <c r="M24" s="2">
-        <f t="shared" si="3"/>
+      <c r="M45" s="2">
+        <f t="shared" si="11"/>
         <v>1.35768</v>
       </c>
-      <c r="N24" s="2">
-        <f t="shared" si="4"/>
+      <c r="N45" s="2">
+        <f t="shared" si="12"/>
         <v>0.29913800000000001</v>
       </c>
     </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="J25" s="2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J46" s="2">
         <v>5</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K46" s="2">
         <v>1.7805100000000001E-4</v>
       </c>
-      <c r="L25" s="2">
-        <f t="shared" si="2"/>
+      <c r="L46" s="2">
+        <f t="shared" si="10"/>
         <v>0.38520100000000002</v>
       </c>
-      <c r="M25" s="2">
-        <f t="shared" si="3"/>
+      <c r="M46" s="2">
+        <f t="shared" si="11"/>
         <v>1.6971000000000001</v>
       </c>
-      <c r="N25" s="2">
-        <f t="shared" si="4"/>
+      <c r="N46" s="2">
+        <f t="shared" si="12"/>
         <v>0.37392250000000005</v>
       </c>
     </row>
-    <row r="26" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="J26" s="2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J47" s="2">
         <v>6</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K47" s="2">
         <v>1.4931999999999999E-4</v>
       </c>
-      <c r="L26" s="2">
-        <f t="shared" si="2"/>
+      <c r="L47" s="2">
+        <f t="shared" si="10"/>
         <v>0.46224120000000007</v>
       </c>
-      <c r="M26" s="2">
-        <f t="shared" si="3"/>
+      <c r="M47" s="2">
+        <f t="shared" si="11"/>
         <v>2.0365200000000003</v>
       </c>
-      <c r="N26" s="2">
-        <f t="shared" si="4"/>
+      <c r="N47" s="2">
+        <f t="shared" si="12"/>
         <v>0.44870700000000002</v>
       </c>
     </row>
-    <row r="27" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="J27" s="2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J48" s="2">
         <v>7</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K48" s="2">
         <v>1.2868800000000001E-4</v>
       </c>
-      <c r="L27" s="2">
-        <f t="shared" si="2"/>
+      <c r="L48" s="2">
+        <f t="shared" si="10"/>
         <v>0.53928140000000002</v>
       </c>
-      <c r="M27" s="2">
-        <f t="shared" si="3"/>
+      <c r="M48" s="2">
+        <f t="shared" si="11"/>
         <v>2.3759399999999999</v>
       </c>
-      <c r="N27" s="2">
-        <f t="shared" si="4"/>
+      <c r="N48" s="2">
+        <f t="shared" si="12"/>
         <v>0.5234915</v>
-      </c>
-    </row>
-    <row r="28" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="J28" s="2">
-        <v>8</v>
-      </c>
-      <c r="K28" s="2">
-        <v>1.1314700000000001E-4</v>
-      </c>
-      <c r="L28" s="2">
-        <f t="shared" si="2"/>
-        <v>0.61632160000000002</v>
-      </c>
-      <c r="M28" s="2">
-        <f t="shared" si="3"/>
-        <v>2.71536</v>
-      </c>
-      <c r="N28" s="2">
-        <f t="shared" si="4"/>
-        <v>0.59827600000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="J29" s="2">
-        <v>9</v>
-      </c>
-      <c r="K29" s="2">
-        <v>1.0101499999999999E-4</v>
-      </c>
-      <c r="L29" s="2">
-        <f t="shared" si="2"/>
-        <v>0.69336180000000003</v>
-      </c>
-      <c r="M29" s="2">
-        <f t="shared" si="3"/>
-        <v>3.0547800000000001</v>
-      </c>
-      <c r="N29" s="2">
-        <f t="shared" si="4"/>
-        <v>0.67306050000000006</v>
-      </c>
-    </row>
-    <row r="30" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="J30" s="2">
-        <v>10</v>
-      </c>
-      <c r="K30" s="4">
-        <v>9.1280799999999995E-5</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0.77040200000000003</v>
-      </c>
-      <c r="M30" s="2">
-        <v>3.3942000000000001</v>
-      </c>
-      <c r="N30" s="2">
-        <v>0.74784499999999998</v>
-      </c>
-    </row>
-    <row r="32" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="I32" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I33" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="J33" s="2">
-        <v>0</v>
-      </c>
-      <c r="K33" s="2">
-        <v>0.693326</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J34" s="2">
-        <v>1</v>
-      </c>
-      <c r="K34" s="2">
-        <v>8.4076300000000001E-4</v>
-      </c>
-      <c r="M34" s="2">
-        <f t="shared" ref="M34:M42" si="5">3.18313*J34/10</f>
-        <v>0.31831299999999996</v>
-      </c>
-      <c r="N34" s="2">
-        <f t="shared" ref="N34:N42" si="6">0.507621*J34/10</f>
-        <v>5.0762099999999998E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J35" s="2">
-        <v>2</v>
-      </c>
-      <c r="K35" s="2">
-        <v>4.3115299999999998E-4</v>
-      </c>
-      <c r="M35" s="2">
-        <f t="shared" si="5"/>
-        <v>0.63662599999999991</v>
-      </c>
-      <c r="N35" s="2">
-        <f t="shared" si="6"/>
-        <v>0.1015242</v>
-      </c>
-    </row>
-    <row r="36" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J36" s="2">
-        <v>3</v>
-      </c>
-      <c r="K36" s="2">
-        <v>2.91532E-4</v>
-      </c>
-      <c r="M36" s="2">
-        <f t="shared" si="5"/>
-        <v>0.95493899999999987</v>
-      </c>
-      <c r="N36" s="2">
-        <f t="shared" si="6"/>
-        <v>0.15228630000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J37" s="2">
-        <v>4</v>
-      </c>
-      <c r="K37" s="2">
-        <v>2.20795E-4</v>
-      </c>
-      <c r="M37" s="2">
-        <f t="shared" si="5"/>
-        <v>1.2732519999999998</v>
-      </c>
-      <c r="N37" s="2">
-        <f t="shared" si="6"/>
-        <v>0.20304839999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J38" s="2">
-        <v>5</v>
-      </c>
-      <c r="K38" s="2">
-        <v>1.77954E-4</v>
-      </c>
-      <c r="M38" s="2">
-        <f t="shared" si="5"/>
-        <v>1.5915649999999999</v>
-      </c>
-      <c r="N38" s="2">
-        <f t="shared" si="6"/>
-        <v>0.25381049999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J39" s="2">
-        <v>6</v>
-      </c>
-      <c r="K39" s="2">
-        <v>1.4919099999999999E-4</v>
-      </c>
-      <c r="M39" s="2">
-        <f t="shared" si="5"/>
-        <v>1.9098779999999997</v>
-      </c>
-      <c r="N39" s="2">
-        <f t="shared" si="6"/>
-        <v>0.30457260000000003</v>
-      </c>
-    </row>
-    <row r="40" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J40" s="2">
-        <v>7</v>
-      </c>
-      <c r="K40" s="2">
-        <v>1.2852499999999999E-4</v>
-      </c>
-      <c r="M40" s="2">
-        <f t="shared" si="5"/>
-        <v>2.2281909999999998</v>
-      </c>
-      <c r="N40" s="2">
-        <f t="shared" si="6"/>
-        <v>0.3553347</v>
-      </c>
-    </row>
-    <row r="41" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J41" s="2">
-        <v>8</v>
-      </c>
-      <c r="K41" s="2">
-        <v>1.1294999999999999E-4</v>
-      </c>
-      <c r="M41" s="2">
-        <f t="shared" si="5"/>
-        <v>2.5465039999999997</v>
-      </c>
-      <c r="N41" s="2">
-        <f t="shared" si="6"/>
-        <v>0.40609679999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J42" s="2">
-        <v>9</v>
-      </c>
-      <c r="K42" s="2">
-        <v>1.00789E-4</v>
-      </c>
-      <c r="M42" s="2">
-        <f t="shared" si="5"/>
-        <v>2.8648169999999995</v>
-      </c>
-      <c r="N42" s="2">
-        <f t="shared" si="6"/>
-        <v>0.45685890000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J43" s="2">
-        <v>10</v>
-      </c>
-      <c r="K43" s="4">
-        <v>9.1024299999999995E-5</v>
-      </c>
-      <c r="M43" s="2">
-        <v>3.1831299999999998</v>
-      </c>
-      <c r="N43" s="2">
-        <v>0.50762099999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I45" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I46" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="J46" s="2">
-        <v>0</v>
-      </c>
-      <c r="K46" s="2">
-        <v>0.693326</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J47" s="2">
-        <v>1</v>
-      </c>
-      <c r="K47" s="2">
-        <v>8.4061599999999998E-4</v>
-      </c>
-      <c r="M47" s="2">
-        <f t="shared" ref="M47:M55" si="7">3.07495*J47/10</f>
-        <v>0.30749499999999996</v>
-      </c>
-      <c r="N47" s="2">
-        <f t="shared" ref="N47:N55" si="8">0.387487*J47/10</f>
-        <v>3.8748700000000004E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J48" s="2">
-        <v>2</v>
-      </c>
-      <c r="K48" s="2">
-        <v>4.3111499999999998E-4</v>
-      </c>
-      <c r="M48" s="2">
-        <f t="shared" si="7"/>
-        <v>0.61498999999999993</v>
-      </c>
-      <c r="N48" s="2">
-        <f t="shared" si="8"/>
-        <v>7.7497400000000008E-2</v>
       </c>
     </row>
     <row r="49" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J49" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K49" s="2">
-        <v>2.91515E-4</v>
+        <v>1.1314700000000001E-4</v>
+      </c>
+      <c r="L49" s="2">
+        <f t="shared" si="10"/>
+        <v>0.61632160000000002</v>
       </c>
       <c r="M49" s="2">
-        <f t="shared" si="7"/>
-        <v>0.922485</v>
+        <f t="shared" si="11"/>
+        <v>2.71536</v>
       </c>
       <c r="N49" s="2">
-        <f t="shared" si="8"/>
-        <v>0.11624609999999999</v>
+        <f t="shared" si="12"/>
+        <v>0.59827600000000003</v>
       </c>
     </row>
     <row r="50" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J50" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K50" s="2">
-        <v>2.20781E-4</v>
+        <v>1.0101499999999999E-4</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" si="10"/>
+        <v>0.69336180000000003</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" si="7"/>
-        <v>1.2299799999999999</v>
+        <f t="shared" si="11"/>
+        <v>3.0547800000000001</v>
       </c>
       <c r="N50" s="2">
-        <f t="shared" si="8"/>
-        <v>0.15499480000000002</v>
+        <f t="shared" si="12"/>
+        <v>0.67306050000000006</v>
       </c>
     </row>
     <row r="51" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J51" s="2">
-        <v>5</v>
-      </c>
-      <c r="K51" s="2">
-        <v>1.7793799999999999E-4</v>
+        <v>10</v>
+      </c>
+      <c r="K51" s="4">
+        <v>9.1280799999999995E-5</v>
+      </c>
+      <c r="L51" s="2">
+        <v>0.77040200000000003</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="7"/>
-        <v>1.5374749999999999</v>
+        <v>3.3942000000000001</v>
       </c>
       <c r="N51" s="2">
-        <f t="shared" si="8"/>
-        <v>0.19374350000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J52" s="2">
-        <v>6</v>
-      </c>
-      <c r="K52" s="2">
-        <v>1.4916699999999999E-4</v>
-      </c>
-      <c r="M52" s="2">
-        <f t="shared" si="7"/>
-        <v>1.84497</v>
-      </c>
-      <c r="N52" s="2">
-        <f t="shared" si="8"/>
-        <v>0.23249219999999998</v>
+        <v>0.74784499999999998</v>
       </c>
     </row>
     <row r="53" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J53" s="2">
-        <v>7</v>
-      </c>
-      <c r="K53" s="2">
-        <v>1.2849399999999999E-4</v>
-      </c>
-      <c r="M53" s="2">
-        <f t="shared" si="7"/>
-        <v>2.1524649999999999</v>
-      </c>
-      <c r="N53" s="2">
-        <f t="shared" si="8"/>
-        <v>0.27124090000000001</v>
+      <c r="I53" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I54" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="J54" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K54" s="2">
-        <v>1.12911E-4</v>
-      </c>
-      <c r="M54" s="2">
-        <f t="shared" si="7"/>
-        <v>2.4599599999999997</v>
-      </c>
-      <c r="N54" s="2">
-        <f t="shared" si="8"/>
-        <v>0.30998960000000003</v>
+        <v>0.693326</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J55" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K55" s="2">
-        <v>1.00739E-4</v>
+        <v>8.4076300000000001E-4</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="7"/>
-        <v>2.767455</v>
+        <f t="shared" ref="M55:M63" si="13">3.18313*J55/10</f>
+        <v>0.31831299999999996</v>
       </c>
       <c r="N55" s="2">
-        <f t="shared" si="8"/>
-        <v>0.34873830000000006</v>
+        <f t="shared" ref="N55:N63" si="14">0.507621*J55/10</f>
+        <v>5.0762099999999998E-2</v>
       </c>
     </row>
     <row r="56" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J56" s="2">
-        <v>10</v>
-      </c>
-      <c r="K56" s="4">
-        <v>9.0964600000000007E-5</v>
+        <v>2</v>
+      </c>
+      <c r="K56" s="2">
+        <v>4.3115299999999998E-4</v>
       </c>
       <c r="M56" s="2">
-        <v>3.0749499999999999</v>
+        <f t="shared" si="13"/>
+        <v>0.63662599999999991</v>
       </c>
       <c r="N56" s="2">
-        <v>0.38748700000000003</v>
+        <f t="shared" si="14"/>
+        <v>0.1015242</v>
+      </c>
+    </row>
+    <row r="57" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J57" s="2">
+        <v>3</v>
+      </c>
+      <c r="K57" s="2">
+        <v>2.91532E-4</v>
+      </c>
+      <c r="M57" s="2">
+        <f t="shared" si="13"/>
+        <v>0.95493899999999987</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="14"/>
+        <v>0.15228630000000001</v>
       </c>
     </row>
     <row r="58" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I58" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>118</v>
+      <c r="J58" s="2">
+        <v>4</v>
+      </c>
+      <c r="K58" s="2">
+        <v>2.20795E-4</v>
+      </c>
+      <c r="M58" s="2">
+        <f t="shared" si="13"/>
+        <v>1.2732519999999998</v>
+      </c>
+      <c r="N58" s="2">
+        <f t="shared" si="14"/>
+        <v>0.20304839999999999</v>
       </c>
     </row>
     <row r="59" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I59" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="J59" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K59" s="2">
-        <v>0.693326</v>
-      </c>
-      <c r="L59" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N59" s="2" t="s">
-        <v>121</v>
+        <v>1.77954E-4</v>
+      </c>
+      <c r="M59" s="2">
+        <f t="shared" si="13"/>
+        <v>1.5915649999999999</v>
+      </c>
+      <c r="N59" s="2">
+        <f t="shared" si="14"/>
+        <v>0.25381049999999999</v>
       </c>
     </row>
     <row r="60" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J60" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K60" s="2">
-        <v>8.4035499999999999E-4</v>
+        <v>1.4919099999999999E-4</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" ref="M60:M68" si="9">3.02188*J60/10</f>
-        <v>0.30218800000000001</v>
+        <f t="shared" si="13"/>
+        <v>1.9098779999999997</v>
       </c>
       <c r="N60" s="2">
-        <f t="shared" ref="N60:N68" si="10">0.327437*J60/10</f>
-        <v>3.2743700000000001E-2</v>
+        <f t="shared" si="14"/>
+        <v>0.30457260000000003</v>
       </c>
     </row>
     <row r="61" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J61" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K61" s="2">
-        <v>4.3105900000000002E-4</v>
+        <v>1.2852499999999999E-4</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" si="9"/>
-        <v>0.60437600000000002</v>
+        <f t="shared" si="13"/>
+        <v>2.2281909999999998</v>
       </c>
       <c r="N61" s="2">
-        <f t="shared" si="10"/>
-        <v>6.5487400000000001E-2</v>
+        <f t="shared" si="14"/>
+        <v>0.3553347</v>
       </c>
     </row>
     <row r="62" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J62" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K62" s="2">
-        <v>2.91494E-4</v>
+        <v>1.1294999999999999E-4</v>
       </c>
       <c r="M62" s="2">
-        <f t="shared" si="9"/>
-        <v>0.90656400000000004</v>
+        <f t="shared" si="13"/>
+        <v>2.5465039999999997</v>
       </c>
       <c r="N62" s="2">
-        <f t="shared" si="10"/>
-        <v>9.8231099999999988E-2</v>
+        <f t="shared" si="14"/>
+        <v>0.40609679999999998</v>
       </c>
     </row>
     <row r="63" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J63" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K63" s="2">
-        <v>2.20771E-4</v>
+        <v>1.00789E-4</v>
       </c>
       <c r="M63" s="2">
-        <f t="shared" si="9"/>
-        <v>1.208752</v>
+        <f t="shared" si="13"/>
+        <v>2.8648169999999995</v>
       </c>
       <c r="N63" s="2">
-        <f t="shared" si="10"/>
-        <v>0.1309748</v>
+        <f t="shared" si="14"/>
+        <v>0.45685890000000001</v>
       </c>
     </row>
     <row r="64" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J64" s="2">
-        <v>5</v>
-      </c>
-      <c r="K64" s="2">
-        <v>1.77935E-4</v>
+        <v>10</v>
+      </c>
+      <c r="K64" s="4">
+        <v>9.1024299999999995E-5</v>
       </c>
       <c r="M64" s="2">
-        <f t="shared" si="9"/>
-        <v>1.5109399999999999</v>
+        <v>3.1831299999999998</v>
       </c>
       <c r="N64" s="2">
-        <f t="shared" si="10"/>
-        <v>0.16371849999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J65" s="2">
-        <v>6</v>
-      </c>
-      <c r="K65" s="2">
-        <v>1.49166E-4</v>
-      </c>
-      <c r="M65" s="2">
-        <f t="shared" si="9"/>
-        <v>1.8131280000000001</v>
-      </c>
-      <c r="N65" s="2">
-        <f t="shared" si="10"/>
-        <v>0.19646219999999998</v>
+        <v>0.50762099999999999</v>
       </c>
     </row>
     <row r="66" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J66" s="2">
-        <v>7</v>
-      </c>
-      <c r="K66" s="2">
-        <v>1.28493E-4</v>
-      </c>
-      <c r="M66" s="2">
-        <f t="shared" si="9"/>
-        <v>2.115316</v>
-      </c>
-      <c r="N66" s="2">
-        <f t="shared" si="10"/>
-        <v>0.22920590000000002</v>
+      <c r="I66" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I67" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="J67" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K67" s="2">
-        <v>1.1291E-4</v>
-      </c>
-      <c r="M67" s="2">
-        <f t="shared" si="9"/>
-        <v>2.4175040000000001</v>
-      </c>
-      <c r="N67" s="2">
-        <f t="shared" si="10"/>
-        <v>0.2619496</v>
+        <v>0.693326</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N67" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J68" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K68" s="2">
-        <v>1.0073699999999999E-4</v>
+        <v>8.4061599999999998E-4</v>
       </c>
       <c r="M68" s="2">
-        <f t="shared" si="9"/>
-        <v>2.7196919999999998</v>
+        <f t="shared" ref="M68:M76" si="15">3.07495*J68/10</f>
+        <v>0.30749499999999996</v>
       </c>
       <c r="N68" s="2">
-        <f t="shared" si="10"/>
-        <v>0.29469329999999994</v>
+        <f t="shared" ref="N68:N76" si="16">0.387487*J68/10</f>
+        <v>3.8748700000000004E-2</v>
       </c>
     </row>
     <row r="69" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J69" s="2">
-        <v>10</v>
-      </c>
-      <c r="K69" s="4">
-        <v>9.0960900000000005E-5</v>
+        <v>2</v>
+      </c>
+      <c r="K69" s="2">
+        <v>4.3111499999999998E-4</v>
       </c>
       <c r="M69" s="2">
-        <v>3.0218799999999999</v>
+        <f t="shared" si="15"/>
+        <v>0.61498999999999993</v>
       </c>
       <c r="N69" s="2">
-        <v>0.32743699999999998</v>
+        <f t="shared" si="16"/>
+        <v>7.7497400000000008E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J70" s="2">
+        <v>3</v>
+      </c>
+      <c r="K70" s="2">
+        <v>2.91515E-4</v>
+      </c>
+      <c r="M70" s="2">
+        <f t="shared" si="15"/>
+        <v>0.922485</v>
+      </c>
+      <c r="N70" s="2">
+        <f t="shared" si="16"/>
+        <v>0.11624609999999999</v>
       </c>
     </row>
     <row r="71" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I71" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>118</v>
+      <c r="J71" s="2">
+        <v>4</v>
+      </c>
+      <c r="K71" s="2">
+        <v>2.20781E-4</v>
+      </c>
+      <c r="M71" s="2">
+        <f t="shared" si="15"/>
+        <v>1.2299799999999999</v>
+      </c>
+      <c r="N71" s="2">
+        <f t="shared" si="16"/>
+        <v>0.15499480000000002</v>
       </c>
     </row>
     <row r="72" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I72" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="J72" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K72" s="2">
-        <v>0.693326</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N72" s="2" t="s">
-        <v>121</v>
+        <v>1.7793799999999999E-4</v>
+      </c>
+      <c r="M72" s="2">
+        <f t="shared" si="15"/>
+        <v>1.5374749999999999</v>
+      </c>
+      <c r="N72" s="2">
+        <f t="shared" si="16"/>
+        <v>0.19374350000000001</v>
       </c>
     </row>
     <row r="73" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J73" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K73" s="2">
-        <v>8.3983599999999995E-4</v>
+        <v>1.4916699999999999E-4</v>
       </c>
       <c r="M73" s="2">
-        <f t="shared" ref="M73:M81" si="11">2.98542*J73/10</f>
-        <v>0.29854199999999997</v>
+        <f t="shared" si="15"/>
+        <v>1.84497</v>
       </c>
       <c r="N73" s="2">
-        <f t="shared" ref="N73:N81" si="12">0.297459*J73/10</f>
-        <v>2.9745899999999999E-2</v>
+        <f t="shared" si="16"/>
+        <v>0.23249219999999998</v>
       </c>
     </row>
     <row r="74" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J74" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K74" s="2">
-        <v>4.3094299999999998E-4</v>
+        <v>1.2849399999999999E-4</v>
       </c>
       <c r="M74" s="2">
-        <f t="shared" si="11"/>
-        <v>0.59708399999999995</v>
+        <f t="shared" si="15"/>
+        <v>2.1524649999999999</v>
       </c>
       <c r="N74" s="2">
-        <f t="shared" si="12"/>
-        <v>5.9491799999999997E-2</v>
+        <f t="shared" si="16"/>
+        <v>0.27124090000000001</v>
       </c>
     </row>
     <row r="75" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J75" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K75" s="2">
-        <v>2.9145000000000001E-4</v>
+        <v>1.12911E-4</v>
       </c>
       <c r="M75" s="2">
-        <f t="shared" si="11"/>
-        <v>0.89562600000000003</v>
+        <f t="shared" si="15"/>
+        <v>2.4599599999999997</v>
       </c>
       <c r="N75" s="2">
-        <f t="shared" si="12"/>
-        <v>8.9237700000000003E-2</v>
+        <f t="shared" si="16"/>
+        <v>0.30998960000000003</v>
       </c>
     </row>
     <row r="76" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J76" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K76" s="2">
-        <v>2.20752E-4</v>
+        <v>1.00739E-4</v>
       </c>
       <c r="M76" s="2">
-        <f t="shared" si="11"/>
-        <v>1.1941679999999999</v>
+        <f t="shared" si="15"/>
+        <v>2.767455</v>
       </c>
       <c r="N76" s="2">
-        <f t="shared" si="12"/>
-        <v>0.11898359999999999</v>
+        <f t="shared" si="16"/>
+        <v>0.34873830000000006</v>
       </c>
     </row>
     <row r="77" spans="9:14" x14ac:dyDescent="0.2">
       <c r="J77" s="2">
+        <v>10</v>
+      </c>
+      <c r="K77" s="4">
+        <v>9.0964600000000007E-5</v>
+      </c>
+      <c r="M77" s="2">
+        <v>3.0749499999999999</v>
+      </c>
+      <c r="N77" s="2">
+        <v>0.38748700000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I79" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I80" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J80" s="2">
+        <v>0</v>
+      </c>
+      <c r="K80" s="2">
+        <v>0.693326</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J81" s="2">
+        <v>1</v>
+      </c>
+      <c r="K81" s="2">
+        <v>8.4035499999999999E-4</v>
+      </c>
+      <c r="M81" s="2">
+        <f t="shared" ref="M81:M89" si="17">3.02188*J81/10</f>
+        <v>0.30218800000000001</v>
+      </c>
+      <c r="N81" s="2">
+        <f t="shared" ref="N81:N89" si="18">0.327437*J81/10</f>
+        <v>3.2743700000000001E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J82" s="2">
+        <v>2</v>
+      </c>
+      <c r="K82" s="2">
+        <v>4.3105900000000002E-4</v>
+      </c>
+      <c r="M82" s="2">
+        <f t="shared" si="17"/>
+        <v>0.60437600000000002</v>
+      </c>
+      <c r="N82" s="2">
+        <f t="shared" si="18"/>
+        <v>6.5487400000000001E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J83" s="2">
+        <v>3</v>
+      </c>
+      <c r="K83" s="2">
+        <v>2.91494E-4</v>
+      </c>
+      <c r="M83" s="2">
+        <f t="shared" si="17"/>
+        <v>0.90656400000000004</v>
+      </c>
+      <c r="N83" s="2">
+        <f t="shared" si="18"/>
+        <v>9.8231099999999988E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J84" s="2">
+        <v>4</v>
+      </c>
+      <c r="K84" s="2">
+        <v>2.20771E-4</v>
+      </c>
+      <c r="M84" s="2">
+        <f t="shared" si="17"/>
+        <v>1.208752</v>
+      </c>
+      <c r="N84" s="2">
+        <f t="shared" si="18"/>
+        <v>0.1309748</v>
+      </c>
+    </row>
+    <row r="85" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J85" s="2">
         <v>5</v>
       </c>
-      <c r="K77" s="2">
+      <c r="K85" s="2">
+        <v>1.77935E-4</v>
+      </c>
+      <c r="M85" s="2">
+        <f t="shared" si="17"/>
+        <v>1.5109399999999999</v>
+      </c>
+      <c r="N85" s="2">
+        <f t="shared" si="18"/>
+        <v>0.16371849999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J86" s="2">
+        <v>6</v>
+      </c>
+      <c r="K86" s="2">
+        <v>1.49166E-4</v>
+      </c>
+      <c r="M86" s="2">
+        <f t="shared" si="17"/>
+        <v>1.8131280000000001</v>
+      </c>
+      <c r="N86" s="2">
+        <f t="shared" si="18"/>
+        <v>0.19646219999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J87" s="2">
+        <v>7</v>
+      </c>
+      <c r="K87" s="2">
+        <v>1.28493E-4</v>
+      </c>
+      <c r="M87" s="2">
+        <f t="shared" si="17"/>
+        <v>2.115316</v>
+      </c>
+      <c r="N87" s="2">
+        <f t="shared" si="18"/>
+        <v>0.22920590000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J88" s="2">
+        <v>8</v>
+      </c>
+      <c r="K88" s="2">
+        <v>1.1291E-4</v>
+      </c>
+      <c r="M88" s="2">
+        <f t="shared" si="17"/>
+        <v>2.4175040000000001</v>
+      </c>
+      <c r="N88" s="2">
+        <f t="shared" si="18"/>
+        <v>0.2619496</v>
+      </c>
+    </row>
+    <row r="89" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J89" s="2">
+        <v>9</v>
+      </c>
+      <c r="K89" s="2">
+        <v>1.0073699999999999E-4</v>
+      </c>
+      <c r="M89" s="2">
+        <f t="shared" si="17"/>
+        <v>2.7196919999999998</v>
+      </c>
+      <c r="N89" s="2">
+        <f t="shared" si="18"/>
+        <v>0.29469329999999994</v>
+      </c>
+    </row>
+    <row r="90" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J90" s="2">
+        <v>10</v>
+      </c>
+      <c r="K90" s="4">
+        <v>9.0960900000000005E-5</v>
+      </c>
+      <c r="M90" s="2">
+        <v>3.0218799999999999</v>
+      </c>
+      <c r="N90" s="2">
+        <v>0.32743699999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I92" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="93" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I93" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J93" s="2">
+        <v>0</v>
+      </c>
+      <c r="K93" s="2">
+        <v>0.693326</v>
+      </c>
+      <c r="L93" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M93" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N93" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J94" s="2">
+        <v>1</v>
+      </c>
+      <c r="K94" s="2">
+        <v>8.3983599999999995E-4</v>
+      </c>
+      <c r="M94" s="2">
+        <f t="shared" ref="M94:M102" si="19">2.98542*J94/10</f>
+        <v>0.29854199999999997</v>
+      </c>
+      <c r="N94" s="2">
+        <f t="shared" ref="N94:N102" si="20">0.297459*J94/10</f>
+        <v>2.9745899999999999E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J95" s="2">
+        <v>2</v>
+      </c>
+      <c r="K95" s="2">
+        <v>4.3094299999999998E-4</v>
+      </c>
+      <c r="M95" s="2">
+        <f t="shared" si="19"/>
+        <v>0.59708399999999995</v>
+      </c>
+      <c r="N95" s="2">
+        <f t="shared" si="20"/>
+        <v>5.9491799999999997E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="J96" s="2">
+        <v>3</v>
+      </c>
+      <c r="K96" s="2">
+        <v>2.9145000000000001E-4</v>
+      </c>
+      <c r="M96" s="2">
+        <f t="shared" si="19"/>
+        <v>0.89562600000000003</v>
+      </c>
+      <c r="N96" s="2">
+        <f t="shared" si="20"/>
+        <v>8.9237700000000003E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J97" s="2">
+        <v>4</v>
+      </c>
+      <c r="K97" s="2">
+        <v>2.20752E-4</v>
+      </c>
+      <c r="M97" s="2">
+        <f t="shared" si="19"/>
+        <v>1.1941679999999999</v>
+      </c>
+      <c r="N97" s="2">
+        <f t="shared" si="20"/>
+        <v>0.11898359999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J98" s="2">
+        <v>5</v>
+      </c>
+      <c r="K98" s="2">
         <v>1.7792599999999999E-4</v>
       </c>
-      <c r="M77" s="2">
-        <f t="shared" si="11"/>
+      <c r="M98" s="2">
+        <f t="shared" si="19"/>
         <v>1.49271</v>
       </c>
-      <c r="N77" s="2">
-        <f t="shared" si="12"/>
+      <c r="N98" s="2">
+        <f t="shared" si="20"/>
         <v>0.14872949999999999</v>
       </c>
     </row>
-    <row r="78" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J78" s="2">
+    <row r="99" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J99" s="2">
         <v>6</v>
       </c>
-      <c r="K78" s="2">
+      <c r="K99" s="2">
         <v>1.4916300000000001E-4</v>
       </c>
-      <c r="M78" s="2">
-        <f t="shared" si="11"/>
+      <c r="M99" s="2">
+        <f t="shared" si="19"/>
         <v>1.7912520000000001</v>
       </c>
-      <c r="N78" s="2">
-        <f t="shared" si="12"/>
+      <c r="N99" s="2">
+        <f t="shared" si="20"/>
         <v>0.17847540000000001</v>
       </c>
     </row>
-    <row r="79" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J79" s="2">
+    <row r="100" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J100" s="2">
         <v>7</v>
       </c>
-      <c r="K79" s="2">
+      <c r="K100" s="2">
         <v>1.28493E-4</v>
       </c>
-      <c r="M79" s="2">
-        <f t="shared" si="11"/>
+      <c r="M100" s="2">
+        <f t="shared" si="19"/>
         <v>2.0897939999999999</v>
       </c>
-      <c r="N79" s="2">
-        <f t="shared" si="12"/>
+      <c r="N100" s="2">
+        <f t="shared" si="20"/>
         <v>0.2082213</v>
       </c>
     </row>
-    <row r="80" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="J80" s="2">
+    <row r="101" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J101" s="2">
         <v>8</v>
       </c>
-      <c r="K80" s="2">
+      <c r="K101" s="2">
         <v>1.12911E-4</v>
       </c>
-      <c r="M80" s="2">
-        <f t="shared" si="11"/>
+      <c r="M101" s="2">
+        <f t="shared" si="19"/>
         <v>2.3883359999999998</v>
       </c>
-      <c r="N80" s="2">
-        <f t="shared" si="12"/>
+      <c r="N101" s="2">
+        <f t="shared" si="20"/>
         <v>0.23796719999999999</v>
       </c>
     </row>
-    <row r="81" spans="10:14" x14ac:dyDescent="0.2">
-      <c r="J81" s="2">
+    <row r="102" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J102" s="2">
         <v>9</v>
       </c>
-      <c r="K81" s="2">
+      <c r="K102" s="2">
         <v>1.00739E-4</v>
       </c>
-      <c r="M81" s="2">
-        <f t="shared" si="11"/>
+      <c r="M102" s="2">
+        <f t="shared" si="19"/>
         <v>2.6868780000000001</v>
       </c>
-      <c r="N81" s="2">
-        <f t="shared" si="12"/>
+      <c r="N102" s="2">
+        <f t="shared" si="20"/>
         <v>0.26771309999999998</v>
       </c>
     </row>
-    <row r="82" spans="10:14" x14ac:dyDescent="0.2">
-      <c r="J82" s="2">
+    <row r="103" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J103" s="2">
         <v>10</v>
       </c>
-      <c r="K82" s="4">
+      <c r="K103" s="4">
         <v>9.0963899999999998E-5</v>
       </c>
-      <c r="M82" s="2">
+      <c r="M103" s="2">
         <v>2.98542</v>
       </c>
-      <c r="N82" s="2">
+      <c r="N103" s="2">
         <v>0.29745899999999997</v>
       </c>
     </row>

</xml_diff>